<commit_message>
Database updates for final runs + TEMBA tests
</commit_message>
<xml_diff>
--- a/Inputs/ARES_Africa/African_hydro_dams.xlsx
+++ b/Inputs/ARES_Africa/African_hydro_dams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DispaSET-SideTools\Inputs\ARES_Africa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2230D129-4DEC-41E1-ACE8-08A23DD096CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622CAF1E-FDA5-42BC-BD2B-A3013AF34D8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="690" yWindow="4545" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1005" yWindow="1215" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydro Dams" sheetId="1" r:id="rId1"/>
@@ -1191,8 +1191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B118" sqref="B2:B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2034,7 +2034,7 @@
         <v>53.44</v>
       </c>
       <c r="I25" s="4">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="J25" s="4">
         <v>-2.9347219999999998</v>
@@ -2069,7 +2069,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="I26" s="4">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="J26" s="4">
         <v>-3.898603</v>
@@ -3971,7 +3971,7 @@
         <v>4.6399999999999997</v>
       </c>
       <c r="I82" s="4">
-        <v>8.8000000000000007</v>
+        <v>248.8</v>
       </c>
       <c r="J82" s="4">
         <v>31.355149000000001</v>

</xml_diff>

<commit_message>
Minor adjustments and new plotting features
</commit_message>
<xml_diff>
--- a/Inputs/ARES_Africa/African_hydro_dams.xlsx
+++ b/Inputs/ARES_Africa/African_hydro_dams.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DispaSET-SideTools\Inputs\ARES_Africa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622CAF1E-FDA5-42BC-BD2B-A3013AF34D8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8801125E-C144-4ED6-8E3F-A3153EEC179C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1005" yWindow="1215" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6240" yWindow="3420" windowWidth="14820" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydro Dams" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="233">
   <si>
     <t>Country</t>
   </si>
@@ -161,9 +161,6 @@
     <t>Calueque</t>
   </si>
   <si>
-    <t>Kwanza</t>
-  </si>
-  <si>
     <t>Lomaum</t>
   </si>
   <si>
@@ -179,9 +176,6 @@
     <t>Mbakaou</t>
   </si>
   <si>
-    <t>Djerem</t>
-  </si>
-  <si>
     <t>Song Loulou</t>
   </si>
   <si>
@@ -209,9 +203,6 @@
     <t>Inga I</t>
   </si>
   <si>
-    <t>Van Deuren</t>
-  </si>
-  <si>
     <t>Inga II</t>
   </si>
   <si>
@@ -227,9 +218,6 @@
     <t>N'Seke</t>
   </si>
   <si>
-    <t>Lualaba</t>
-  </si>
-  <si>
     <t>N'Zilo I and II</t>
   </si>
   <si>
@@ -245,15 +233,9 @@
     <t>Djiboloho</t>
   </si>
   <si>
-    <t>Wele</t>
-  </si>
-  <si>
     <t>Tchimbele</t>
   </si>
   <si>
-    <t>M'Bei</t>
-  </si>
-  <si>
     <t>Grand Poubara</t>
   </si>
   <si>
@@ -281,9 +263,6 @@
     <t>High Aswan</t>
   </si>
   <si>
-    <t>Koka</t>
-  </si>
-  <si>
     <t>Awash I</t>
   </si>
   <si>
@@ -302,9 +281,6 @@
     <t>Gilgel Gibe I</t>
   </si>
   <si>
-    <t>Gilgel Gibe</t>
-  </si>
-  <si>
     <t>Gilgel Gibe II</t>
   </si>
   <si>
@@ -449,9 +425,6 @@
     <t xml:space="preserve">Kabalega </t>
   </si>
   <si>
-    <t>Wambabya</t>
-  </si>
-  <si>
     <t>Kanungu</t>
   </si>
   <si>
@@ -497,9 +470,6 @@
     <t>Muvembe</t>
   </si>
   <si>
-    <t>Maziba</t>
-  </si>
-  <si>
     <t>Al Massira</t>
   </si>
   <si>
@@ -512,9 +482,6 @@
     <t>Al Wahda</t>
   </si>
   <si>
-    <t>Ouergha</t>
-  </si>
-  <si>
     <t>Allal Al Fassi</t>
   </si>
   <si>
@@ -524,9 +491,6 @@
     <t>Bin El Ouidane</t>
   </si>
   <si>
-    <t>El Abid</t>
-  </si>
-  <si>
     <t>Afourer</t>
   </si>
   <si>
@@ -536,9 +500,6 @@
     <t>Lakhdar</t>
   </si>
   <si>
-    <t>Inaouene</t>
-  </si>
-  <si>
     <t>Idriss I</t>
   </si>
   <si>
@@ -548,9 +509,6 @@
     <t>El Kansera</t>
   </si>
   <si>
-    <t>Beht</t>
-  </si>
-  <si>
     <t>Mohammed V</t>
   </si>
   <si>
@@ -560,24 +518,15 @@
     <t>Tanafit El Borj</t>
   </si>
   <si>
-    <t>Oum Er Rbia</t>
-  </si>
-  <si>
     <t>Sidi Said Maachou</t>
   </si>
   <si>
     <t>Oued El Makhazine</t>
   </si>
   <si>
-    <t>Loukkos</t>
-  </si>
-  <si>
     <t>Moulay Youssef</t>
   </si>
   <si>
-    <t>Tessaout</t>
-  </si>
-  <si>
     <t>Imfout</t>
   </si>
   <si>
@@ -587,9 +536,6 @@
     <t>Sidi Salem</t>
   </si>
   <si>
-    <t>Medjerba</t>
-  </si>
-  <si>
     <t>Nebeur</t>
   </si>
   <si>
@@ -611,9 +557,6 @@
     <t>Ubangi</t>
   </si>
   <si>
-    <t>Inkisi</t>
-  </si>
-  <si>
     <t>Ogooue</t>
   </si>
   <si>
@@ -675,6 +618,120 @@
   </si>
   <si>
     <t>Tulila</t>
+  </si>
+  <si>
+    <t>El Hammam</t>
+  </si>
+  <si>
+    <t>El Tleta</t>
+  </si>
+  <si>
+    <t>Uggug Iragen</t>
+  </si>
+  <si>
+    <t>Fodda</t>
+  </si>
+  <si>
+    <t>Cuanza</t>
+  </si>
+  <si>
+    <t>Bandoca</t>
+  </si>
+  <si>
+    <t>Dange</t>
+  </si>
+  <si>
+    <t>Chicapa</t>
+  </si>
+  <si>
+    <t>Benue</t>
+  </si>
+  <si>
+    <t>Kansi</t>
+  </si>
+  <si>
+    <t>Benito</t>
+  </si>
+  <si>
+    <t>Awash</t>
+  </si>
+  <si>
+    <t>Gibir Shet</t>
+  </si>
+  <si>
+    <t>Mabo</t>
+  </si>
+  <si>
+    <t>Abangassa</t>
+  </si>
+  <si>
+    <t>Victoria Nile</t>
+  </si>
+  <si>
+    <t>Sagana</t>
+  </si>
+  <si>
+    <t>Alhandar</t>
+  </si>
+  <si>
+    <t>Ouerrha</t>
+  </si>
+  <si>
+    <t>L'abid</t>
+  </si>
+  <si>
+    <t>Er-Rbia</t>
+  </si>
+  <si>
+    <t>Baht</t>
+  </si>
+  <si>
+    <t>Abiod</t>
+  </si>
+  <si>
+    <t>Tassaout</t>
+  </si>
+  <si>
+    <t>Loukos</t>
+  </si>
+  <si>
+    <t>Oum Er R'bia</t>
+  </si>
+  <si>
+    <t>Tensift</t>
+  </si>
+  <si>
+    <t>Draa</t>
+  </si>
+  <si>
+    <t>Kivu</t>
+  </si>
+  <si>
+    <t>Madjerda</t>
+  </si>
+  <si>
+    <t>Mellegue</t>
+  </si>
+  <si>
+    <t>Sejnane</t>
+  </si>
+  <si>
+    <t>Medjerda</t>
+  </si>
+  <si>
+    <t>Sidi Bou Heurtma</t>
+  </si>
+  <si>
+    <t>Mubuku</t>
+  </si>
+  <si>
+    <t>Kanyabaha</t>
+  </si>
+  <si>
+    <t>Muvumba</t>
+  </si>
+  <si>
+    <t>Rovuma</t>
   </si>
 </sst>
 </file>
@@ -1191,8 +1248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B118" sqref="B2:B124"/>
+    <sheetView tabSelected="1" topLeftCell="B80" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:K124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,9 +1376,11 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C4" s="1"/>
+        <v>183</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>195</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1350,9 +1409,11 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C5" s="1"/>
+        <v>184</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1379,9 +1440,11 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C6" s="1"/>
+        <v>185</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>196</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1410,9 +1473,11 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C7" s="1"/>
+        <v>186</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1439,9 +1504,11 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C8" s="4"/>
+        <v>187</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>198</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1473,7 +1540,7 @@
         <v>39</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>194</v>
+        <v>40</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>34</v>
@@ -1508,7 +1575,7 @@
         <v>41</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>34</v>
@@ -1542,7 +1609,7 @@
         <v>33</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>42</v>
+        <v>199</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>34</v>
@@ -1577,7 +1644,7 @@
         <v>35</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>42</v>
+        <v>199</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>34</v>
@@ -1612,7 +1679,7 @@
         <v>37</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>34</v>
@@ -1644,10 +1711,10 @@
         <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>34</v>
@@ -1682,7 +1749,7 @@
         <v>38</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>34</v>
@@ -1717,7 +1784,7 @@
         <v>36</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>34</v>
@@ -1749,9 +1816,11 @@
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C17" s="4"/>
+        <v>188</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>202</v>
+      </c>
       <c r="D17" s="4" t="s">
         <v>34</v>
       </c>
@@ -1780,13 +1849,13 @@
         <v>23</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E18" s="4">
         <v>1982</v>
@@ -1811,13 +1880,13 @@
         <v>23</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E19" s="4">
         <v>1991</v>
@@ -1826,7 +1895,7 @@
         <v>5</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H19" s="4">
         <v>1.53</v>
@@ -1846,13 +1915,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="E20" s="4">
         <v>1953</v>
@@ -1881,13 +1950,13 @@
         <v>18</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21" s="4">
         <v>1971</v>
@@ -1914,13 +1983,13 @@
         <v>18</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="E22" s="4">
         <v>1980</v>
@@ -1949,11 +2018,13 @@
         <v>18</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="C23" s="4"/>
+        <v>189</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>203</v>
+      </c>
       <c r="D23" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4">
@@ -1978,13 +2049,13 @@
         <v>19</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E24" s="4">
         <v>1976</v>
@@ -1993,7 +2064,7 @@
         <v>5</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H24" s="4">
         <v>0.01</v>
@@ -2013,13 +2084,13 @@
         <v>20</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E25" s="4">
         <v>2011</v>
@@ -2048,13 +2119,13 @@
         <v>20</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E26" s="4">
         <v>1974</v>
@@ -2080,16 +2151,16 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E27" s="4">
         <v>1972</v>
@@ -2115,16 +2186,16 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>59</v>
-      </c>
       <c r="C28" s="4" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E28" s="4">
         <v>1977</v>
@@ -2150,16 +2221,16 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E29" s="4">
         <v>1949</v>
@@ -2185,16 +2256,16 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4">
@@ -2214,16 +2285,16 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E31" s="4">
         <v>1956</v>
@@ -2249,16 +2320,16 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E32" s="4">
         <v>1953</v>
@@ -2284,16 +2355,16 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E33" s="4">
         <v>1959</v>
@@ -2319,16 +2390,16 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E34" s="4">
         <v>1989</v>
@@ -2354,16 +2425,16 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E35" s="4">
         <v>1955</v>
@@ -2389,16 +2460,16 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E36" s="4">
         <v>2017</v>
@@ -2407,7 +2478,7 @@
         <v>20</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H36" s="4">
         <v>0.14000000000000001</v>
@@ -2427,13 +2498,13 @@
         <v>24</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E37" s="4">
         <v>1994</v>
@@ -2458,13 +2529,13 @@
         <v>24</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E38" s="4">
         <v>1970</v>
@@ -2493,13 +2564,13 @@
         <v>24</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E39" s="4">
         <v>2008</v>
@@ -2524,13 +2595,13 @@
         <v>24</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E40" s="4">
         <v>1933</v>
@@ -2559,13 +2630,13 @@
         <v>21</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>70</v>
+        <v>205</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E41" s="4">
         <v>2008</v>
@@ -2592,20 +2663,20 @@
         <v>25</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>82</v>
+        <v>206</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4">
         <v>5</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H42" s="4">
         <v>167.06</v>
@@ -2625,20 +2696,20 @@
         <v>25</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>82</v>
+        <v>206</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4">
         <v>5</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H43" s="4">
         <v>0.03</v>
@@ -2658,13 +2729,13 @@
         <v>25</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="E44" s="4">
         <v>2010</v>
@@ -2689,13 +2760,13 @@
         <v>25</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E45" s="4">
         <v>1973</v>
@@ -2724,13 +2795,13 @@
         <v>25</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E46" s="4">
         <v>1973</v>
@@ -2759,13 +2830,13 @@
         <v>25</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E47" s="4">
         <v>2017</v>
@@ -2774,7 +2845,7 @@
         <v>110</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H47" s="4"/>
       <c r="I47" s="4">
@@ -2792,13 +2863,13 @@
         <v>25</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>89</v>
+        <v>207</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E48" s="4">
         <v>2004</v>
@@ -2827,13 +2898,13 @@
         <v>25</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>89</v>
+        <v>207</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E49" s="4">
         <v>2004</v>
@@ -2860,13 +2931,13 @@
         <v>25</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>89</v>
+        <v>207</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E50" s="4">
         <v>2004</v>
@@ -2895,13 +2966,13 @@
         <v>25</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E51" s="4">
         <v>1960</v>
@@ -2930,13 +3001,13 @@
         <v>25</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E52" s="4">
         <v>2009</v>
@@ -2965,13 +3036,13 @@
         <v>25</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E53" s="4">
         <v>2001</v>
@@ -2998,13 +3069,13 @@
         <v>22</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E54" s="4">
         <v>2013</v>
@@ -3031,13 +3102,13 @@
         <v>22</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>72</v>
+        <v>208</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E55" s="4">
         <v>1980</v>
@@ -3066,11 +3137,13 @@
         <v>22</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C56" s="4"/>
       <c r="D56" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4">
@@ -3095,13 +3168,13 @@
         <v>26</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E57" s="4">
         <v>1978</v>
@@ -3130,13 +3203,13 @@
         <v>26</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E58" s="4">
         <v>1974</v>
@@ -3165,13 +3238,13 @@
         <v>26</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E59" s="4">
         <v>1987</v>
@@ -3200,13 +3273,13 @@
         <v>26</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E60" s="4">
         <v>1968</v>
@@ -3235,13 +3308,13 @@
         <v>26</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E61" s="4">
         <v>1980</v>
@@ -3270,13 +3343,13 @@
         <v>26</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>110</v>
+        <v>210</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E62" s="4">
         <v>1954</v>
@@ -3305,13 +3378,13 @@
         <v>26</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E63" s="4">
         <v>2009</v>
@@ -3338,13 +3411,13 @@
         <v>26</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>101</v>
+        <v>211</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E64" s="4">
         <v>2009</v>
@@ -3353,7 +3426,7 @@
         <v>10</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H64" s="4"/>
       <c r="I64" s="4">
@@ -3371,13 +3444,13 @@
         <v>26</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E65" s="4">
         <v>1991</v>
@@ -3406,11 +3479,13 @@
         <v>31</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="C66" s="4"/>
+        <v>152</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>212</v>
+      </c>
       <c r="D66" s="4" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E66" s="4">
         <v>2004</v>
@@ -3439,13 +3514,13 @@
         <v>31</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E67" s="4">
         <v>1979</v>
@@ -3474,13 +3549,13 @@
         <v>31</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>159</v>
+        <v>213</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E68" s="4">
         <v>1996</v>
@@ -3509,13 +3584,13 @@
         <v>31</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E69" s="4">
         <v>1990</v>
@@ -3544,13 +3619,13 @@
         <v>31</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>163</v>
+        <v>214</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E70" s="4">
         <v>1953</v>
@@ -3579,13 +3654,13 @@
         <v>31</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E71" s="4">
         <v>1950</v>
@@ -3614,11 +3689,13 @@
         <v>31</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C72" s="4"/>
+        <v>153</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>215</v>
+      </c>
       <c r="D72" s="4" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4">
@@ -3643,13 +3720,13 @@
         <v>31</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>171</v>
+        <v>216</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E73" s="4">
         <v>1935</v>
@@ -3678,13 +3755,13 @@
         <v>31</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E74" s="4">
         <v>1986</v>
@@ -3713,13 +3790,13 @@
         <v>31</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>167</v>
+        <v>217</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E75" s="4">
         <v>1973</v>
@@ -3748,13 +3825,13 @@
         <v>31</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E76" s="4">
         <v>1944</v>
@@ -3783,10 +3860,10 @@
         <v>31</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>4</v>
@@ -3818,13 +3895,13 @@
         <v>31</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>180</v>
+        <v>218</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E78" s="4">
         <v>1969</v>
@@ -3853,13 +3930,13 @@
         <v>31</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>178</v>
+        <v>219</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E79" s="4">
         <v>1979</v>
@@ -3888,13 +3965,13 @@
         <v>31</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>175</v>
+        <v>220</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E80" s="4">
         <v>1929</v>
@@ -3923,13 +4000,13 @@
         <v>31</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E81" s="4">
         <v>2007</v>
@@ -3956,11 +4033,13 @@
         <v>31</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="C82" s="4"/>
+        <v>191</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>221</v>
+      </c>
       <c r="D82" s="4" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E82" s="4"/>
       <c r="F82" s="4">
@@ -3985,11 +4064,13 @@
         <v>31</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C83" s="4"/>
+        <v>192</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>222</v>
+      </c>
       <c r="D83" s="4" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E83" s="4"/>
       <c r="F83" s="4">
@@ -4014,13 +4095,13 @@
         <v>27</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E84" s="4">
         <v>2010</v>
@@ -4029,7 +4110,7 @@
         <v>10</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H84" s="4"/>
       <c r="I84" s="4">
@@ -4047,13 +4128,13 @@
         <v>27</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>112</v>
+        <v>223</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E85" s="4">
         <v>1959</v>
@@ -4062,7 +4143,7 @@
         <v>10</v>
       </c>
       <c r="G85" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H85" s="4"/>
       <c r="I85" s="4">
@@ -4080,13 +4161,13 @@
         <v>27</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E86" s="4">
         <v>2014</v>
@@ -4095,7 +4176,7 @@
         <v>10</v>
       </c>
       <c r="G86" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H86" s="4">
         <v>3.26</v>
@@ -4115,13 +4196,13 @@
         <v>27</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E87" s="4">
         <v>2014</v>
@@ -4146,13 +4227,13 @@
         <v>27</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E88" s="4">
         <v>1958</v>
@@ -4179,13 +4260,13 @@
         <v>27</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E89" s="4">
         <v>1989</v>
@@ -4212,13 +4293,13 @@
         <v>28</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E90" s="4">
         <v>2006</v>
@@ -4243,13 +4324,13 @@
         <v>29</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E91" s="4">
         <v>1937</v>
@@ -4278,13 +4359,13 @@
         <v>29</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E92" s="4">
         <v>1964</v>
@@ -4313,13 +4394,13 @@
         <v>29</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E93" s="4">
         <v>2009</v>
@@ -4348,13 +4429,13 @@
         <v>29</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E94" s="4">
         <v>1966</v>
@@ -4383,13 +4464,13 @@
         <v>29</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E95" s="4">
         <v>1925</v>
@@ -4418,13 +4499,13 @@
         <v>29</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E96" s="4">
         <v>2017</v>
@@ -4451,9 +4532,11 @@
         <v>32</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="C97" s="4"/>
+        <v>168</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>224</v>
+      </c>
       <c r="D97" s="4" t="s">
         <v>4</v>
       </c>
@@ -4480,9 +4563,11 @@
         <v>32</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="C98" s="4"/>
+        <v>169</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>169</v>
+      </c>
       <c r="D98" s="4" t="s">
         <v>4</v>
       </c>
@@ -4509,9 +4594,11 @@
         <v>32</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="C99" s="4"/>
+        <v>167</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>225</v>
+      </c>
       <c r="D99" s="4" t="s">
         <v>4</v>
       </c>
@@ -4540,9 +4627,11 @@
         <v>32</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="C100" s="4"/>
+        <v>170</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>226</v>
+      </c>
       <c r="D100" s="4" t="s">
         <v>4</v>
       </c>
@@ -4567,10 +4656,10 @@
         <v>32</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>184</v>
+        <v>227</v>
       </c>
       <c r="D101" s="4" t="s">
         <v>4</v>
@@ -4602,9 +4691,11 @@
         <v>32</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="C102" s="3"/>
+        <v>193</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>228</v>
+      </c>
       <c r="D102" s="4" t="s">
         <v>4</v>
       </c>
@@ -4631,13 +4722,13 @@
         <v>30</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>110</v>
+        <v>229</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E103" s="4">
         <v>2009</v>
@@ -4662,13 +4753,13 @@
         <v>30</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>110</v>
+        <v>210</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E104" s="4">
         <v>2012</v>
@@ -4697,13 +4788,13 @@
         <v>30</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>138</v>
+        <v>102</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E105" s="4">
         <v>2013</v>
@@ -4730,13 +4821,13 @@
         <v>30</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E106" s="4">
         <v>2011</v>
@@ -4761,13 +4852,13 @@
         <v>30</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>110</v>
+        <v>210</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E107" s="4">
         <v>2003</v>
@@ -4794,13 +4885,13 @@
         <v>30</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>148</v>
+        <v>230</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E108" s="4">
         <v>2008</v>
@@ -4825,11 +4916,13 @@
         <v>30</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C109" s="4"/>
+        <v>133</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="D109" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E109" s="4">
         <v>2011</v>
@@ -4856,13 +4949,13 @@
         <v>30</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E110" s="4">
         <v>1950</v>
@@ -4887,13 +4980,13 @@
         <v>30</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E111" s="4">
         <v>2009</v>
@@ -4918,13 +5011,13 @@
         <v>30</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>154</v>
+        <v>231</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E112" s="4">
         <v>2017</v>
@@ -4949,13 +5042,13 @@
         <v>30</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>76</v>
+        <v>210</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E113" s="4">
         <v>1954</v>
@@ -4982,13 +5075,13 @@
         <v>30</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E114" s="4">
         <v>2012</v>
@@ -5013,13 +5106,13 @@
         <v>30</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E115" s="4">
         <v>2017</v>
@@ -5044,13 +5137,13 @@
         <v>30</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E116" s="4">
         <v>2017</v>
@@ -5075,13 +5168,13 @@
         <v>30</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E117" s="4">
         <v>2017</v>
@@ -5103,16 +5196,16 @@
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E118" s="4">
         <v>1964</v>
@@ -5138,16 +5231,16 @@
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E119" s="4">
         <v>1975</v>
@@ -5173,16 +5266,16 @@
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E120" s="4">
         <v>2000</v>
@@ -5208,16 +5301,16 @@
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E121" s="4">
         <v>1980</v>
@@ -5243,16 +5336,16 @@
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E122" s="4">
         <v>1966</v>
@@ -5278,16 +5371,16 @@
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B123" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B123" s="4" t="s">
-        <v>133</v>
-      </c>
       <c r="C123" s="4" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E123" s="4">
         <v>1994</v>
@@ -5313,14 +5406,16 @@
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="C124" s="1"/>
+        <v>194</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>232</v>
+      </c>
       <c r="D124" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
@@ -5340,7 +5435,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A2:I2 A9:G16 A4:A8 A17 A23 A57:G81 A56 A82:A83 A102 A124 A84:G101 D4:D8 I84:I101 I103:I123 I57:I81 I9:I16 A3:G3 I3 D17 D23 D56 D82:D83 D102 A18:G22 I18:I22 A24:G55 I24:I55 H3:H123 D124 A103:G123">
+  <conditionalFormatting sqref="A2:I2 A4:A8 A17 A23 A57:G81 A56 A82:A83 A102 A124 A84:G101 D4:D8 I84:I101 I103:I123 I57:I81 I9:I16 A3:G3 I3 D17 D23 D56 D82:D83 D102 A18:G22 I18:I22 I24:I55 H3:H123 D124 A103:G123 A9:G16 A24:G55">
     <cfRule type="containsBlanks" dxfId="12" priority="2">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>

</xml_diff>